<commit_message>
Added main file for algorithm (needs debuging and testing)
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="O2">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debuging of DE and GA
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixing of diverse bugs
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed objective to multi objective; default only TAC optimization
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E814E51-7E21-4146-BD12-6A332D372F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14610" windowHeight="6210"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,6 +192,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -226,6 +244,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -401,11 +436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,13 +499,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.9</v>
@@ -479,10 +514,10 @@
         <v>0.1</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -491,10 +526,13 @@
         <v>0.9</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <v>5</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added optional interactive mode to enter variables at the end of the execution
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E814E51-7E21-4146-BD12-6A332D372F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14610" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,23 +191,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -244,23 +226,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,11 +401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,13 +464,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0.9</v>
@@ -514,10 +479,10 @@
         <v>0.1</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -526,13 +491,10 @@
         <v>0.9</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>5</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Pareto front size limit variable
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335C7CD6-7440-4B18-B556-0B6EBCE6828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14610" windowHeight="6210"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>PopSizeGA</t>
   </si>
@@ -50,12 +51,15 @@
   </si>
   <si>
     <t>PerturbationDE</t>
+  </si>
+  <si>
+    <t>ParetoSize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,6 +195,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -226,6 +247,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -401,11 +439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,14 +455,15 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,22 +486,25 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -479,22 +521,28 @@
         <v>0.1</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G2">
         <v>200</v>
       </c>
       <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
         <v>0.5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.9</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>100</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>5</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added objective selection to the algorithm
</commit_message>
<xml_diff>
--- a/data/AlgorithmParameter.xlsx
+++ b/data/AlgorithmParameter.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335C7CD6-7440-4B18-B556-0B6EBCE6828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3F320-BCA5-4294-B889-3CC0D9A64F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>PopSizeGA</t>
   </si>
@@ -54,6 +54,24 @@
   </si>
   <si>
     <t>ParetoSize</t>
+  </si>
+  <si>
+    <t>OF_options</t>
+  </si>
+  <si>
+    <t>TAC</t>
+  </si>
+  <si>
+    <t>GHG</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>OFs</t>
   </si>
 </sst>
 </file>
@@ -98,10 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -440,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +480,7 @@
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,25 +511,31 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>0.9</v>
@@ -543,6 +566,26 @@
       </c>
       <c r="M2">
         <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>